<commit_message>
testing with different precision
</commit_message>
<xml_diff>
--- a/ExcelScore/PSO_5D.xlsx
+++ b/ExcelScore/PSO_5D.xlsx
@@ -655,49 +655,49 @@
         </is>
       </c>
       <c r="B2" s="4" t="n">
-        <v>1.2e-09</v>
+        <v>8.799999999999999e-09</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>4.5e-09</v>
+        <v>5.5e-09</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>3.4e-09</v>
+        <v>6.6e-09</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>5.2e-09</v>
+        <v>4.8e-09</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>1.8e-09</v>
+        <v>8.200000000000001e-09</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>4e-09</v>
+        <v>6e-09</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>4.2e-09</v>
+        <v>5.8e-09</v>
       </c>
       <c r="I2" s="4" t="n">
-        <v>1.4e-09</v>
+        <v>8.600000000000001e-09</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>4.4e-09</v>
+        <v>5.600000000000001e-09</v>
       </c>
       <c r="K2" s="4" t="n">
-        <v>4.1e-10</v>
+        <v>9.59e-09</v>
       </c>
       <c r="L2" s="4" t="n">
-        <v>8e-10</v>
+        <v>9.2e-09</v>
       </c>
       <c r="M2" s="4" t="n">
-        <v>2.6e-09</v>
+        <v>7.4e-09</v>
       </c>
       <c r="N2" s="4" t="n">
-        <v>5e-10</v>
+        <v>9.500000000000001e-09</v>
       </c>
       <c r="O2" s="4" t="n">
-        <v>7.3e-09</v>
+        <v>2.7e-09</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>2.3e-09</v>
+        <v>7.699999999999999e-09</v>
       </c>
       <c r="R2" s="5">
         <f>FLOOR(-LOG10(B2),1)</f>
@@ -767,49 +767,49 @@
         </is>
       </c>
       <c r="B3" s="4" t="n">
-        <v>4.1e-09</v>
+        <v>5.9e-09</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>3.9e-09</v>
+        <v>6.1e-09</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>1.6e-09</v>
+        <v>8.400000000000001e-09</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>8.1e-10</v>
+        <v>9.19e-09</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>4.9e-09</v>
+        <v>5.1e-09</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>3.4e-09</v>
+        <v>6.6e-09</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>3.3e-09</v>
+        <v>6.7e-09</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>1.9e-09</v>
+        <v>8.1e-09</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>3.1e-09</v>
+        <v>6.900000000000001e-09</v>
       </c>
       <c r="K3" s="4" t="n">
-        <v>2.7e-09</v>
+        <v>7.3e-09</v>
       </c>
       <c r="L3" s="4" t="n">
-        <v>1.3e-09</v>
+        <v>8.7e-09</v>
       </c>
       <c r="M3" s="4" t="n">
-        <v>1.7e-09</v>
+        <v>8.3e-09</v>
       </c>
       <c r="N3" s="4" t="n">
-        <v>2.5e-09</v>
+        <v>7.500000000000001e-09</v>
       </c>
       <c r="O3" s="4" t="n">
-        <v>4.8e-10</v>
+        <v>9.52e-09</v>
       </c>
       <c r="P3" s="4" t="n">
-        <v>3.3e-09</v>
+        <v>6.7e-09</v>
       </c>
       <c r="R3" s="5">
         <f>FLOOR(-LOG10(B3),1)</f>
@@ -879,49 +879,49 @@
         </is>
       </c>
       <c r="B4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>5.2e-09</v>
+        <v>4.8e-09</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>2.1e-09</v>
+        <v>7.9e-09</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>2.7e-09</v>
+        <v>7.3e-09</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>7.5e-10</v>
+        <v>9.25e-09</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>3.2e-09</v>
+        <v>6.8e-09</v>
       </c>
       <c r="L4" s="4" t="n">
-        <v>4.3e-09</v>
+        <v>5.700000000000001e-09</v>
       </c>
       <c r="M4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="N4" s="4" t="n">
-        <v>1.5e-10</v>
+        <v>9.850000000000001e-09</v>
       </c>
       <c r="O4" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="P4" s="4" t="n">
-        <v>1.5e-09</v>
+        <v>8.5e-09</v>
       </c>
       <c r="R4" s="5">
         <f>FLOOR(-LOG10(B4),1)</f>
@@ -991,49 +991,49 @@
         </is>
       </c>
       <c r="B5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>7.7e-10</v>
+        <v>9.230000000000001e-09</v>
       </c>
       <c r="I5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="L5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="M5" s="4" t="n">
-        <v>3</v>
+        <v>3.00000001</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="O5" s="4" t="n">
-        <v>11</v>
+        <v>11.00000001</v>
       </c>
       <c r="P5" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="R5" s="5">
         <f>FLOOR(-LOG10(B5),1)</f>
@@ -1103,49 +1103,49 @@
         </is>
       </c>
       <c r="B6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="K6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="M6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="N6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="O6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="P6" s="4" t="n">
-        <v>1e-08</v>
+        <v>0</v>
       </c>
       <c r="R6" s="5">
         <f>FLOOR(-LOG10(B6),1)</f>
@@ -1215,49 +1215,49 @@
         </is>
       </c>
       <c r="B7" s="4" t="n">
-        <v>7.8e-10</v>
+        <v>9.220000000000001e-09</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>1.1e-09</v>
+        <v>8.9e-09</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>2e-09</v>
+        <v>8e-09</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>4.1e-09</v>
+        <v>5.9e-09</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>4.7e-09</v>
+        <v>5.3e-09</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>2.9e-10</v>
+        <v>9.710000000000001e-09</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>3.7e-09</v>
+        <v>6.3e-09</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>1.9e-10</v>
+        <v>9.81e-09</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>3.3e-10</v>
+        <v>9.67e-09</v>
       </c>
       <c r="K7" s="4" t="n">
-        <v>2.5e-09</v>
+        <v>7.500000000000001e-09</v>
       </c>
       <c r="L7" s="4" t="n">
-        <v>4.5e-09</v>
+        <v>5.5e-09</v>
       </c>
       <c r="M7" s="4" t="n">
-        <v>4.1e-09</v>
+        <v>5.9e-09</v>
       </c>
       <c r="N7" s="4" t="n">
-        <v>2.1e-09</v>
+        <v>7.9e-09</v>
       </c>
       <c r="O7" s="4" t="n">
-        <v>5.4e-10</v>
+        <v>9.46e-09</v>
       </c>
       <c r="P7" s="4" t="n">
-        <v>1.8e-09</v>
+        <v>8.200000000000001e-09</v>
       </c>
       <c r="R7" s="5">
         <f>FLOOR(-LOG10(B7),1)</f>
@@ -1327,49 +1327,49 @@
         </is>
       </c>
       <c r="B8" s="4" t="n">
-        <v>9.500000000000001e-09</v>
+        <v>4.999999999999995e-10</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>0.13</v>
+        <v>0.13000001</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>0.38</v>
+        <v>0.38000001</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0.21</v>
+        <v>0.21000001</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>9.500000000000001e-09</v>
+        <v>4.999999999999995e-10</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>9.6e-10</v>
+        <v>9.04e-09</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>5.5e-09</v>
+        <v>4.500000000000001e-09</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>2.8e-10</v>
+        <v>9.72e-09</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>6.6e-09</v>
+        <v>3.4e-09</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>6.8e-09</v>
+        <v>3.200000000000001e-09</v>
       </c>
       <c r="L8" s="4" t="n">
-        <v>0.33</v>
+        <v>0.33000001</v>
       </c>
       <c r="M8" s="4" t="n">
-        <v>2.6e-09</v>
+        <v>7.4e-09</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>1.4</v>
+        <v>1.40000001</v>
       </c>
       <c r="O8" s="4" t="n">
-        <v>9.1e-09</v>
+        <v>8.999999999999998e-10</v>
       </c>
       <c r="P8" s="4" t="n">
-        <v>0.14</v>
+        <v>0.14000001</v>
       </c>
       <c r="R8" s="5">
         <f>FLOOR(-LOG10(B8),1)</f>
@@ -1439,49 +1439,49 @@
         </is>
       </c>
       <c r="B9" s="4" t="n">
-        <v>0.034</v>
+        <v>0.03400001</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>0.034</v>
+        <v>0.03400001</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>0.027</v>
+        <v>0.02700001</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>0.05</v>
+        <v>0.05000001</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>0.038</v>
+        <v>0.03800001</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>0.033</v>
+        <v>0.03300001</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>0.049</v>
+        <v>0.04900001</v>
       </c>
       <c r="I9" s="4" t="n">
-        <v>0.023</v>
+        <v>0.02300001</v>
       </c>
       <c r="J9" s="4" t="n">
-        <v>0.066</v>
+        <v>0.06600001</v>
       </c>
       <c r="K9" s="4" t="n">
-        <v>0.063</v>
+        <v>0.06300001</v>
       </c>
       <c r="L9" s="4" t="n">
-        <v>0.0074</v>
+        <v>0.00740001</v>
       </c>
       <c r="M9" s="4" t="n">
-        <v>0.07099999999999999</v>
+        <v>0.07100000999999999</v>
       </c>
       <c r="N9" s="4" t="n">
-        <v>0.14</v>
+        <v>0.14000001</v>
       </c>
       <c r="O9" s="4" t="n">
-        <v>0.036</v>
+        <v>0.03600001</v>
       </c>
       <c r="P9" s="4" t="n">
-        <v>0.037</v>
+        <v>0.03700001</v>
       </c>
       <c r="R9" s="5">
         <f>FLOOR(-LOG10(B9),1)</f>
@@ -1551,49 +1551,49 @@
         </is>
       </c>
       <c r="B10" s="4" t="n">
-        <v>3.9</v>
+        <v>3.90000001</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>0.014</v>
+        <v>0.01400001</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>0.019</v>
+        <v>0.01900001</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0.024</v>
+        <v>0.02400001</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>1.5e-05</v>
+        <v>1.501e-05</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0.023</v>
+        <v>0.02300001</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.06900001</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>0.089</v>
+        <v>0.08900000999999999</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>0.062</v>
+        <v>0.06200001</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>0.083</v>
+        <v>0.08300001</v>
       </c>
       <c r="L10" s="4" t="n">
-        <v>0.011</v>
+        <v>0.01100001</v>
       </c>
       <c r="M10" s="4" t="n">
-        <v>4.1</v>
+        <v>4.10000001</v>
       </c>
       <c r="N10" s="4" t="n">
-        <v>0.032</v>
+        <v>0.03200001</v>
       </c>
       <c r="O10" s="4" t="n">
-        <v>3.9</v>
+        <v>3.90000001</v>
       </c>
       <c r="P10" s="4" t="n">
-        <v>0.013</v>
+        <v>0.01300001</v>
       </c>
       <c r="R10" s="5">
         <f>FLOOR(-LOG10(B10),1)</f>
@@ -1663,49 +1663,49 @@
         </is>
       </c>
       <c r="B11" s="4" t="n">
-        <v>37</v>
+        <v>37.00000001</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>23</v>
+        <v>23.00000001</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>57</v>
+        <v>57.00000001</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>33</v>
+        <v>33.00000001</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>6.9</v>
+        <v>6.90000001</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>37</v>
+        <v>37.00000001</v>
       </c>
       <c r="H11" s="4" t="n">
-        <v>95</v>
+        <v>95.00000000999999</v>
       </c>
       <c r="I11" s="4" t="n">
-        <v>23</v>
+        <v>23.00000001</v>
       </c>
       <c r="J11" s="4" t="n">
-        <v>110</v>
+        <v>110.00000001</v>
       </c>
       <c r="K11" s="4" t="n">
-        <v>19</v>
+        <v>19.00000001</v>
       </c>
       <c r="L11" s="4" t="n">
-        <v>23</v>
+        <v>23.00000001</v>
       </c>
       <c r="M11" s="4" t="n">
-        <v>140</v>
+        <v>140.00000001</v>
       </c>
       <c r="N11" s="4" t="n">
-        <v>47</v>
+        <v>47.00000001</v>
       </c>
       <c r="O11" s="4" t="n">
-        <v>28</v>
+        <v>28.00000001</v>
       </c>
       <c r="P11" s="4" t="n">
-        <v>27</v>
+        <v>27.00000001</v>
       </c>
       <c r="R11" s="5">
         <f>FLOOR(-LOG10(B11),1)</f>
@@ -1775,49 +1775,49 @@
         </is>
       </c>
       <c r="B12" s="4" t="n">
-        <v>0.025</v>
+        <v>0.02500001</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>0.34</v>
+        <v>0.34000001</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>4.6</v>
+        <v>4.60000001</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>1.6</v>
+        <v>1.60000001</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>0.15</v>
+        <v>0.15000001</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>0.2</v>
+        <v>0.20000001</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>0.96</v>
+        <v>0.96000001</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>0.26</v>
+        <v>0.26000001</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>1.3</v>
+        <v>1.30000001</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>0.36</v>
+        <v>0.36000001</v>
       </c>
       <c r="L12" s="4" t="n">
-        <v>1</v>
+        <v>1.00000001</v>
       </c>
       <c r="M12" s="4" t="n">
-        <v>1.2</v>
+        <v>1.20000001</v>
       </c>
       <c r="N12" s="4" t="n">
-        <v>1.2</v>
+        <v>1.20000001</v>
       </c>
       <c r="O12" s="4" t="n">
-        <v>0.32</v>
+        <v>0.32000001</v>
       </c>
       <c r="P12" s="4" t="n">
-        <v>1.2</v>
+        <v>1.20000001</v>
       </c>
       <c r="R12" s="5">
         <f>FLOOR(-LOG10(B12),1)</f>
@@ -1887,49 +1887,49 @@
         </is>
       </c>
       <c r="B13" s="4" t="n">
-        <v>37</v>
+        <v>37.00000001</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>11</v>
+        <v>11.00000001</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>3.2</v>
+        <v>3.20000001</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>0.37</v>
+        <v>0.37000001</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>0.95</v>
+        <v>0.95000001</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>11</v>
+        <v>11.00000001</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>1.1</v>
+        <v>1.10000001</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>0.038</v>
+        <v>0.03800001</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>12</v>
+        <v>12.00000001</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="L13" s="4" t="n">
-        <v>86</v>
+        <v>86.00000000999999</v>
       </c>
       <c r="M13" s="4" t="n">
-        <v>8.9</v>
+        <v>8.900000010000001</v>
       </c>
       <c r="N13" s="4" t="n">
-        <v>4.7</v>
+        <v>4.70000001</v>
       </c>
       <c r="O13" s="4" t="n">
-        <v>3</v>
+        <v>3.00000001</v>
       </c>
       <c r="P13" s="4" t="n">
-        <v>50</v>
+        <v>50.00000001</v>
       </c>
       <c r="R13" s="5">
         <f>FLOOR(-LOG10(B13),1)</f>
@@ -1999,49 +1999,49 @@
         </is>
       </c>
       <c r="B14" s="4" t="n">
-        <v>4.6</v>
+        <v>4.60000001</v>
       </c>
       <c r="C14" s="4" t="n">
-        <v>19</v>
+        <v>19.00000001</v>
       </c>
       <c r="D14" s="4" t="n">
-        <v>2.8</v>
+        <v>2.80000001</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>11</v>
+        <v>11.00000001</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>0.74</v>
+        <v>0.74000001</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>1</v>
+        <v>1.00000001</v>
       </c>
       <c r="H14" s="4" t="n">
-        <v>16</v>
+        <v>16.00000001</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>3.4</v>
+        <v>3.40000001</v>
       </c>
       <c r="J14" s="4" t="n">
-        <v>5.5</v>
+        <v>5.50000001</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>2.5</v>
+        <v>2.50000001</v>
       </c>
       <c r="L14" s="4" t="n">
-        <v>7.4</v>
+        <v>7.40000001</v>
       </c>
       <c r="M14" s="4" t="n">
-        <v>0.016</v>
+        <v>0.01600001</v>
       </c>
       <c r="N14" s="4" t="n">
-        <v>3.8</v>
+        <v>3.80000001</v>
       </c>
       <c r="O14" s="4" t="n">
-        <v>5.7</v>
+        <v>5.70000001</v>
       </c>
       <c r="P14" s="4" t="n">
-        <v>13</v>
+        <v>13.00000001</v>
       </c>
       <c r="R14" s="5">
         <f>FLOOR(-LOG10(B14),1)</f>
@@ -2111,49 +2111,49 @@
         </is>
       </c>
       <c r="B15" s="4" t="n">
-        <v>2.4e-05</v>
+        <v>2.401e-05</v>
       </c>
       <c r="C15" s="4" t="n">
-        <v>2.1e-06</v>
+        <v>2.11e-06</v>
       </c>
       <c r="D15" s="4" t="n">
-        <v>3e-06</v>
+        <v>3.01e-06</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>2.7e-05</v>
+        <v>2.701e-05</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>1.9e-05</v>
+        <v>1.901e-05</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>2.3e-05</v>
+        <v>2.301e-05</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>2.3e-05</v>
+        <v>2.301e-05</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>2.4e-05</v>
+        <v>2.401e-05</v>
       </c>
       <c r="J15" s="4" t="n">
-        <v>2.4e-05</v>
+        <v>2.401e-05</v>
       </c>
       <c r="K15" s="4" t="n">
-        <v>2.9e-05</v>
+        <v>2.901e-05</v>
       </c>
       <c r="L15" s="4" t="n">
-        <v>3.6e-06</v>
+        <v>3.61e-06</v>
       </c>
       <c r="M15" s="4" t="n">
-        <v>8.600000000000001e-06</v>
+        <v>8.610000000000001e-06</v>
       </c>
       <c r="N15" s="4" t="n">
-        <v>2.2e-06</v>
+        <v>2.21e-06</v>
       </c>
       <c r="O15" s="4" t="n">
-        <v>2.8e-05</v>
+        <v>2.801e-05</v>
       </c>
       <c r="P15" s="4" t="n">
-        <v>3.6e-05</v>
+        <v>3.601e-05</v>
       </c>
       <c r="R15" s="5">
         <f>FLOOR(-LOG10(B15),1)</f>
@@ -2223,49 +2223,49 @@
         </is>
       </c>
       <c r="B16" s="4" t="n">
-        <v>4</v>
+        <v>4.00000001</v>
       </c>
       <c r="C16" s="4" t="n">
-        <v>5</v>
+        <v>5.00000001</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>5</v>
+        <v>5.00000001</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>5</v>
+        <v>5.00000001</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>4</v>
+        <v>4.00000001</v>
       </c>
       <c r="J16" s="4" t="n">
-        <v>0.99</v>
+        <v>0.99000001</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>4</v>
+        <v>4.00000001</v>
       </c>
       <c r="M16" s="4" t="n">
-        <v>7</v>
+        <v>7.00000001</v>
       </c>
       <c r="N16" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="O16" s="4" t="n">
-        <v>3</v>
+        <v>3.00000001</v>
       </c>
       <c r="P16" s="4" t="n">
-        <v>4</v>
+        <v>4.00000001</v>
       </c>
       <c r="R16" s="5">
         <f>FLOOR(-LOG10(B16),1)</f>
@@ -2335,49 +2335,49 @@
         </is>
       </c>
       <c r="B17" s="4" t="n">
-        <v>0.82</v>
+        <v>0.82000001</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>0.12</v>
+        <v>0.12000001</v>
       </c>
       <c r="D17" s="4" t="n">
-        <v>0.35</v>
+        <v>0.35000001</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0.012</v>
+        <v>0.01200001</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>0.13</v>
+        <v>0.13000001</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0.052</v>
+        <v>0.05200001</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>1.1</v>
+        <v>1.10000001</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>0.78</v>
+        <v>0.7800000100000001</v>
       </c>
       <c r="J17" s="4" t="n">
-        <v>0.016</v>
+        <v>0.01600001</v>
       </c>
       <c r="K17" s="4" t="n">
-        <v>1.3</v>
+        <v>1.30000001</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>0.01</v>
+        <v>0.01000001</v>
       </c>
       <c r="M17" s="4" t="n">
-        <v>0.16</v>
+        <v>0.16000001</v>
       </c>
       <c r="N17" s="4" t="n">
-        <v>0.74</v>
+        <v>0.74000001</v>
       </c>
       <c r="O17" s="4" t="n">
-        <v>0.54</v>
+        <v>0.5400000100000001</v>
       </c>
       <c r="P17" s="4" t="n">
-        <v>0.16</v>
+        <v>0.16000001</v>
       </c>
       <c r="R17" s="5">
         <f>FLOOR(-LOG10(B17),1)</f>
@@ -2447,49 +2447,49 @@
         </is>
       </c>
       <c r="B18" s="4" t="n">
-        <v>0.0021</v>
+        <v>0.00210001</v>
       </c>
       <c r="C18" s="4" t="n">
-        <v>0.53</v>
+        <v>0.5300000100000001</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>1.6e-07</v>
+        <v>1.7e-07</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>0.001</v>
+        <v>0.00100001</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>2.7e-05</v>
+        <v>2.701e-05</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>0.016</v>
+        <v>0.01600001</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>0.17</v>
+        <v>0.17000001</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>1.5e-05</v>
+        <v>1.501e-05</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>0.00047</v>
+        <v>0.00047001</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>0.018</v>
+        <v>0.01800001</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>0.00048</v>
+        <v>0.00048001</v>
       </c>
       <c r="M18" s="4" t="n">
-        <v>0.26</v>
+        <v>0.26000001</v>
       </c>
       <c r="N18" s="4" t="n">
-        <v>0.053</v>
+        <v>0.05300001</v>
       </c>
       <c r="O18" s="4" t="n">
-        <v>1.6e-05</v>
+        <v>1.601e-05</v>
       </c>
       <c r="P18" s="4" t="n">
-        <v>0.00049</v>
+        <v>0.00049001</v>
       </c>
       <c r="R18" s="5">
         <f>FLOOR(-LOG10(B18),1)</f>
@@ -2559,49 +2559,49 @@
         </is>
       </c>
       <c r="B19" s="4" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.07200000999999999</v>
       </c>
       <c r="C19" s="4" t="n">
-        <v>0.089</v>
+        <v>0.08900000999999999</v>
       </c>
       <c r="D19" s="4" t="n">
-        <v>0.14</v>
+        <v>0.14000001</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>0.12</v>
+        <v>0.12000001</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>0.33</v>
+        <v>0.33000001</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>0.012</v>
+        <v>0.01200001</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0.016</v>
+        <v>0.01600001</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0.12</v>
+        <v>0.12000001</v>
       </c>
       <c r="J19" s="4" t="n">
-        <v>0.14</v>
+        <v>0.14000001</v>
       </c>
       <c r="K19" s="4" t="n">
-        <v>0.2</v>
+        <v>0.20000001</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>0.23</v>
+        <v>0.23000001</v>
       </c>
       <c r="M19" s="4" t="n">
-        <v>0.11</v>
+        <v>0.11000001</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>0.033</v>
+        <v>0.03300001</v>
       </c>
       <c r="O19" s="4" t="n">
-        <v>0.79</v>
+        <v>0.7900000100000001</v>
       </c>
       <c r="P19" s="4" t="n">
-        <v>0.11</v>
+        <v>0.11000001</v>
       </c>
       <c r="R19" s="5">
         <f>FLOOR(-LOG10(B19),1)</f>
@@ -2671,49 +2671,49 @@
         </is>
       </c>
       <c r="B20" s="4" t="n">
-        <v>0.06900000000000001</v>
+        <v>0.06900001</v>
       </c>
       <c r="C20" s="4" t="n">
-        <v>0.08699999999999999</v>
+        <v>0.08700000999999999</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>0.19</v>
+        <v>0.19000001</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>0.31</v>
+        <v>0.31000001</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0.34</v>
+        <v>0.34000001</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>0.27</v>
+        <v>0.27000001</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0.15</v>
+        <v>0.15000001</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0.11</v>
+        <v>0.11000001</v>
       </c>
       <c r="J20" s="4" t="n">
-        <v>0.13</v>
+        <v>0.13000001</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.07200000999999999</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>0.13</v>
+        <v>0.13000001</v>
       </c>
       <c r="M20" s="4" t="n">
-        <v>0.33</v>
+        <v>0.33000001</v>
       </c>
       <c r="N20" s="4" t="n">
-        <v>0.061</v>
+        <v>0.06100001</v>
       </c>
       <c r="O20" s="4" t="n">
-        <v>0.25</v>
+        <v>0.25000001</v>
       </c>
       <c r="P20" s="4" t="n">
-        <v>0.2</v>
+        <v>0.20000001</v>
       </c>
       <c r="R20" s="5">
         <f>FLOOR(-LOG10(B20),1)</f>
@@ -2783,49 +2783,49 @@
         </is>
       </c>
       <c r="B21" s="4" t="n">
-        <v>7.4e-10</v>
+        <v>9.26e-09</v>
       </c>
       <c r="C21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="D21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>0.47</v>
+        <v>0.47000001</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="J21" s="4" t="n">
-        <v>4e-09</v>
+        <v>6e-09</v>
       </c>
       <c r="K21" s="4" t="n">
-        <v>1.5e-09</v>
+        <v>8.5e-09</v>
       </c>
       <c r="L21" s="4" t="n">
-        <v>3.9e-09</v>
+        <v>6.1e-09</v>
       </c>
       <c r="M21" s="4" t="n">
-        <v>0.67</v>
+        <v>0.6700000100000001</v>
       </c>
       <c r="N21" s="4" t="n">
-        <v>0.47</v>
+        <v>0.47000001</v>
       </c>
       <c r="O21" s="4" t="n">
-        <v>0.24</v>
+        <v>0.24000001</v>
       </c>
       <c r="P21" s="4" t="n">
-        <v>1.4e-09</v>
+        <v>8.600000000000001e-09</v>
       </c>
       <c r="R21" s="5">
         <f>FLOOR(-LOG10(B21),1)</f>
@@ -2895,49 +2895,49 @@
         </is>
       </c>
       <c r="B22" s="4" t="n">
-        <v>4.6e-09</v>
+        <v>5.4e-09</v>
       </c>
       <c r="C22" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="D22" s="4" t="n">
-        <v>1.8</v>
+        <v>1.80000001</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>4.2</v>
+        <v>4.20000001</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>5.6e-09</v>
+        <v>4.400000000000001e-09</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>0.93</v>
+        <v>0.9300000100000001</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="J22" s="4" t="n">
-        <v>2.5</v>
+        <v>2.50000001</v>
       </c>
       <c r="K22" s="4" t="n">
-        <v>1.2</v>
+        <v>1.20000001</v>
       </c>
       <c r="L22" s="4" t="n">
-        <v>1.2e-09</v>
+        <v>8.799999999999999e-09</v>
       </c>
       <c r="M22" s="4" t="n">
-        <v>1.9</v>
+        <v>1.90000001</v>
       </c>
       <c r="N22" s="4" t="n">
-        <v>0.93</v>
+        <v>0.9300000100000001</v>
       </c>
       <c r="O22" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="P22" s="4" t="n">
-        <v>1.6</v>
+        <v>1.60000001</v>
       </c>
       <c r="R22" s="5">
         <f>FLOOR(-LOG10(B22),1)</f>
@@ -3007,49 +3007,49 @@
         </is>
       </c>
       <c r="B23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="C23" s="4" t="n">
-        <v>5.1</v>
+        <v>5.10000001</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>5.8e-09</v>
+        <v>4.2e-09</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="G23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="J23" s="4" t="n">
-        <v>1.4e-10</v>
+        <v>9.86e-09</v>
       </c>
       <c r="K23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="L23" s="4" t="n">
-        <v>4.8e-10</v>
+        <v>9.52e-09</v>
       </c>
       <c r="M23" s="4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.69000001</v>
       </c>
       <c r="N23" s="4" t="n">
-        <v>2.6</v>
+        <v>2.60000001</v>
       </c>
       <c r="O23" s="4" t="n">
-        <v>3e-09</v>
+        <v>7e-09</v>
       </c>
       <c r="P23" s="4" t="n">
-        <v>2</v>
+        <v>2.00000001</v>
       </c>
       <c r="R23" s="5">
         <f>FLOOR(-LOG10(B23),1)</f>
@@ -3119,49 +3119,49 @@
         </is>
       </c>
       <c r="B24" s="4" t="n">
-        <v>0.027</v>
+        <v>0.02700001</v>
       </c>
       <c r="C24" s="4" t="n">
-        <v>0.6</v>
+        <v>0.60000001</v>
       </c>
       <c r="D24" s="4" t="n">
-        <v>0.2</v>
+        <v>0.20000001</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>0.092</v>
+        <v>0.09200000999999999</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>0.044</v>
+        <v>0.04400001</v>
       </c>
       <c r="G24" s="4" t="n">
-        <v>0.18</v>
+        <v>0.18000001</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>0.72</v>
+        <v>0.72000001</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>0.13</v>
+        <v>0.13000001</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>0.55</v>
+        <v>0.5500000100000001</v>
       </c>
       <c r="K24" s="4" t="n">
-        <v>0.36</v>
+        <v>0.36000001</v>
       </c>
       <c r="L24" s="4" t="n">
-        <v>0.72</v>
+        <v>0.72000001</v>
       </c>
       <c r="M24" s="4" t="n">
-        <v>0.57</v>
+        <v>0.57000001</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>0.097</v>
+        <v>0.09700001</v>
       </c>
       <c r="O24" s="4" t="n">
-        <v>0.082</v>
+        <v>0.08200001</v>
       </c>
       <c r="P24" s="4" t="n">
-        <v>0.76</v>
+        <v>0.7600000100000001</v>
       </c>
       <c r="R24" s="5">
         <f>FLOOR(-LOG10(B24),1)</f>
@@ -3231,49 +3231,49 @@
         </is>
       </c>
       <c r="B25" s="4" t="n">
-        <v>7.3</v>
+        <v>7.30000001</v>
       </c>
       <c r="C25" s="4" t="n">
-        <v>6.6</v>
+        <v>6.60000001</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>9.300000000000001</v>
+        <v>9.300000010000002</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>10</v>
+        <v>10.00000001</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>5.5</v>
+        <v>5.50000001</v>
       </c>
       <c r="G25" s="4" t="n">
-        <v>8.5</v>
+        <v>8.500000010000001</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>2.4</v>
+        <v>2.40000001</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>8.9</v>
+        <v>8.900000010000001</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>8.300000000000001</v>
+        <v>8.300000010000002</v>
       </c>
       <c r="K25" s="4" t="n">
-        <v>6.2</v>
+        <v>6.20000001</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>8.199999999999999</v>
+        <v>8.20000001</v>
       </c>
       <c r="M25" s="4" t="n">
-        <v>6</v>
+        <v>6.00000001</v>
       </c>
       <c r="N25" s="4" t="n">
-        <v>9.800000000000001</v>
+        <v>9.800000010000002</v>
       </c>
       <c r="O25" s="4" t="n">
-        <v>6.7</v>
+        <v>6.70000001</v>
       </c>
       <c r="P25" s="4" t="n">
-        <v>2.1</v>
+        <v>2.10000001</v>
       </c>
       <c r="R25" s="5">
         <f>FLOOR(-LOG10(B25),1)</f>

</xml_diff>